<commit_message>
analysis through DESeq2 and DAVID enrichment
</commit_message>
<xml_diff>
--- a/data/Crabs for RNA analysis.xlsx
+++ b/data/Crabs for RNA analysis.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BBB0ED-A966-E84A-8E49-E9CC59D1A59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,12 +60,6 @@
     <t>pH 7.5</t>
   </si>
   <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Short</t>
-  </si>
-  <si>
     <t>pH 7.8</t>
   </si>
   <si>
@@ -64,12 +70,18 @@
   </si>
   <si>
     <t>Snow Crab Juveniles- m-RNA analysis samples</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,51 +416,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -459,7 +471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -470,7 +482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -481,7 +493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -492,7 +504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -503,7 +515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>5</v>
       </c>
@@ -514,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>6</v>
       </c>
@@ -525,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>7</v>
       </c>
@@ -536,7 +548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>8</v>
       </c>
@@ -547,7 +559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>9</v>
       </c>
@@ -558,7 +570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>10</v>
       </c>
@@ -569,7 +581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>11</v>
       </c>
@@ -580,7 +592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>12</v>
       </c>
@@ -591,7 +603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>13</v>
       </c>
@@ -599,10 +611,10 @@
         <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -610,10 +622,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -621,10 +633,10 @@
         <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -632,10 +644,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>17</v>
       </c>
@@ -643,10 +655,10 @@
         <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -654,10 +666,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -665,10 +677,10 @@
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -676,10 +688,10 @@
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>21</v>
       </c>
@@ -687,10 +699,10 @@
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>22</v>
       </c>
@@ -698,10 +710,10 @@
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>23</v>
       </c>
@@ -709,10 +721,10 @@
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>24</v>
       </c>
@@ -720,10 +732,10 @@
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>25</v>
       </c>
@@ -731,10 +743,10 @@
         <v>8</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>26</v>
       </c>
@@ -742,10 +754,10 @@
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>27</v>
       </c>
@@ -753,10 +765,10 @@
         <v>8</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>28</v>
       </c>
@@ -764,10 +776,10 @@
         <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>29</v>
       </c>
@@ -775,10 +787,10 @@
         <v>8</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>30</v>
       </c>
@@ -786,10 +798,10 @@
         <v>8</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>31</v>
       </c>
@@ -797,10 +809,10 @@
         <v>8</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>32</v>
       </c>
@@ -808,10 +820,10 @@
         <v>8</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>33</v>
       </c>
@@ -819,10 +831,10 @@
         <v>8</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>34</v>
       </c>
@@ -830,10 +842,10 @@
         <v>8</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>35</v>
       </c>
@@ -841,10 +853,10 @@
         <v>8</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>36</v>
       </c>
@@ -852,10 +864,10 @@
         <v>8</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>37</v>
       </c>
@@ -863,10 +875,10 @@
         <v>8</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>38</v>
       </c>
@@ -874,282 +886,282 @@
         <v>8</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>39</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>40</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>41</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>42</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>43</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>44</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>45</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>46</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>47</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>48</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>49</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>50</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>51</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>52</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>53</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>54</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>55</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>56</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>57</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>58</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>59</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>60</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>61</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>62</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>63</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>